<commit_message>
added BOM for USART BOSL converter
</commit_message>
<xml_diff>
--- a/USART_BoSL_Bus/USART_BoSL_Bus_BOM rev 0.1.0.xlsx
+++ b/USART_BoSL_Bus/USART_BoSL_Bus_BOM rev 0.1.0.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20361"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F507979-E452-4B8D-828E-27D1BF96F2F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -18,8 +19,103 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+  <si>
+    <t>Part Number</t>
+  </si>
+  <si>
+    <t>Package Size / Type</t>
+  </si>
+  <si>
+    <t>Schematic Designator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Component </t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>QTY per board</t>
+  </si>
+  <si>
+    <t>Unit Price (USD)</t>
+  </si>
+  <si>
+    <t>Total Price (USD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supplier </t>
+  </si>
+  <si>
+    <t>SMD Resistor</t>
+  </si>
+  <si>
+    <t>SOIC-8</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>https://au.mouser.com/ProductDetail/Texas-Instruments/SN65HVD75DR?qs=X2y4EmDJZOW1Viw5bHgBbQ%3D%3D</t>
+  </si>
+  <si>
+    <t>RS-485 Line Driver</t>
+  </si>
+  <si>
+    <t>SN65HVD75DR</t>
+  </si>
+  <si>
+    <t>https://au.mouser.com/ProductDetail/Amphenol-FCI/54601-906001WPLF?qs=A%252Bwkq3FTowXIf3bXQPL90g%3D%3D</t>
+  </si>
+  <si>
+    <t>6P6C Connector</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>Amphenol 54601</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>0.1" Pin Socket</t>
+  </si>
+  <si>
+    <t>01x06</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>01x08</t>
+  </si>
+  <si>
+    <t>0.1" Pin Header</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>100 Ω</t>
+  </si>
+  <si>
+    <t>R2,R3</t>
+  </si>
+  <si>
+    <t>47 kΩ</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -49,8 +145,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +427,261 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>3.77</v>
+      </c>
+      <c r="H2" s="1">
+        <f>G2*F2</f>
+        <v>3.77</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="H3" s="1">
+        <f>G3*F3</f>
+        <v>0.4</v>
+      </c>
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H4" s="1">
+        <f>G4*F4</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" ref="H5:H8" si="0">G5*F5</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>603</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>603</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added production files fro bosl bus converter
</commit_message>
<xml_diff>
--- a/USART_BoSL_Bus/USART_BoSL_Bus_BOM rev 0.1.0.xlsx
+++ b/USART_BoSL_Bus/USART_BoSL_Bus_BOM rev 0.1.0.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20361"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC42C8B-FF27-4067-B856-1BDCE3217DB6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645D9427-FAC0-4FF4-B665-00267710E6A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>Part Number</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>47 kΩ</t>
+  </si>
+  <si>
+    <t>J4</t>
   </si>
 </sst>
 </file>
@@ -431,7 +434,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,7 +572,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
         <v>24</v>
@@ -626,14 +629,14 @@
         <v>28</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8" s="1">
         <v>0.1</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>